<commit_message>
completed MTP POC target assoc script
</commit_message>
<xml_diff>
--- a/InputFiles/MTP_DataValidation_TargetAssoc_InputFile.xlsx
+++ b/InputFiles/MTP_DataValidation_TargetAssoc_InputFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAC2BEC-5362-414A-9D43-667FE315284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024AFFA6-20C4-4F45-83D4-40E95FD3CFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="targetAssoc" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -97,10 +97,19 @@
     <t>/target/ENSG00000169083/associations</t>
   </si>
   <si>
-    <t>MTP_DataValidation_TargetAssoc_InputFile</t>
-  </si>
-  <si>
-    <t>outputFilename</t>
+    <t>suffix_Url</t>
+  </si>
+  <si>
+    <t>target_ID</t>
+  </si>
+  <si>
+    <t>target_Name</t>
+  </si>
+  <si>
+    <t>PMTLcode</t>
+  </si>
+  <si>
+    <t>diseaseCount</t>
   </si>
 </sst>
 </file>
@@ -118,6 +127,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -363,10 +373,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -375,33 +385,27 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -417,8 +421,56 @@
       <c r="E2" s="1">
         <v>758</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1022</v>
       </c>
     </row>
   </sheetData>
@@ -434,7 +486,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F5"/>
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -539,26 +591,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -781,26 +813,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10D0160D-ABCF-4D5A-A5FB-7B381F923E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6291852C-9D1E-423D-9DD5-FD3E66999552}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3985B68-D08C-48CA-A6A6-31C2BAA63FE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -817,4 +850,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6291852C-9D1E-423D-9DD5-FD3E66999552}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10D0160D-ABCF-4D5A-A5FB-7B381F923E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
all rows in data binding
</commit_message>
<xml_diff>
--- a/InputFiles/MTP_DataValidation_TargetAssoc_InputFile.xlsx
+++ b/InputFiles/MTP_DataValidation_TargetAssoc_InputFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024AFFA6-20C4-4F45-83D4-40E95FD3CFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109DC5AD-50C0-4CBE-8977-82AD7E81202A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="4335" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="targetAssoc" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -373,10 +373,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -424,52 +424,35 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1">
-        <v>2676</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1">
         <v>1022</v>
       </c>
     </row>
@@ -591,6 +574,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -813,27 +816,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10D0160D-ABCF-4D5A-A5FB-7B381F923E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6291852C-9D1E-423D-9DD5-FD3E66999552}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3985B68-D08C-48CA-A6A6-31C2BAA63FE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -850,23 +852,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6291852C-9D1E-423D-9DD5-FD3E66999552}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10D0160D-ABCF-4D5A-A5FB-7B381F923E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>